<commit_message>
file: fixed_backtester.py added - replacing backtest_enhanced_TM
</commit_message>
<xml_diff>
--- a/results/Backtesting Distance vs Strategy.xlsx
+++ b/results/Backtesting Distance vs Strategy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sim\Desktop\Quant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sim\Desktop\Quant\OTC\trading-strategy-automation\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D4227C-109A-44B4-90EC-44A7EFC74013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37E406D-18E1-4E99-B7BA-9007A60A2083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="17" activeTab="23" xr2:uid="{CD23B6F1-1309-401E-B828-5DBBF72A400D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="15" activeTab="22" xr2:uid="{CD23B6F1-1309-401E-B828-5DBBF72A400D}"/>
   </bookViews>
   <sheets>
     <sheet name="AUDNZD" sheetId="1" r:id="rId1"/>
@@ -3816,7 +3816,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" activeCellId="3" sqref="C4 K4 K22 C22"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22135,8 +22135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CE3C66-0FA2-4AA5-ABB8-6808D1636663}">
   <dimension ref="A1:U160"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23070,7 +23070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B51C155D-82F5-40F8-9A0D-C0662100A0E6}">
   <dimension ref="A1:W999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>

</xml_diff>